<commit_message>
Updated invariants of an Encounter for an Event  and generated the output for SML CIFMM-2704
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/encounter-es-1.xlsx
+++ b/output/SharedMedicinesList/encounter-es-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="432">
   <si>
     <t>Path</t>
   </si>
@@ -154,7 +154,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-enc-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Encounter[@moodCode='EVN']</t>
@@ -646,10 +646,6 @@
   </si>
   <si>
     <t>While the encounter is always about the patient, the patient may not actually be known in all contexts of use, and there may be a group of patients that could be anonymous (such as in a group therapy for Alcoholics Anonymous - where the recording of the encounter could be used for billing on the number of people/staff and not important to the context of the specific patients) or alternately in veterinary care a herd of sheep receiving treatment (where the animals are not individually tracked).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-enc-01:The subject shall at least have a reference or an identifier {reference.exists() or identifier.exists()}
-</t>
   </si>
   <si>
     <t>.participation[typeCode=SBJ]/role[classCode=PAT]</t>
@@ -4769,21 +4765,21 @@
         <v>42</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="AJ30" t="s" s="2">
+      <c r="AK30" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AK30" t="s" s="2">
+      <c r="AL30" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AL30" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4806,13 +4802,13 @@
         <v>50</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4863,7 +4859,7 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4881,15 +4877,15 @@
         <v>139</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>209</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4912,13 +4908,13 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="L32" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4969,7 +4965,7 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -4984,7 +4980,7 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
@@ -4995,7 +4991,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5021,10 +5017,10 @@
         <v>134</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>216</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>217</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5075,7 +5071,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5090,18 +5086,18 @@
         <v>138</v>
       </c>
       <c r="AJ33" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL33" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>219</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5207,7 +5203,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5315,7 +5311,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5423,7 +5419,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5449,13 +5445,13 @@
         <v>178</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5484,10 +5480,10 @@
         <v>72</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>42</v>
@@ -5505,7 +5501,7 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5520,18 +5516,18 @@
         <v>42</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5557,10 +5553,10 @@
         <v>155</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5611,7 +5607,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5626,18 +5622,18 @@
         <v>42</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>234</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5660,13 +5656,13 @@
         <v>50</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5717,7 +5713,7 @@
         <v>42</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5732,18 +5728,18 @@
         <v>42</v>
       </c>
       <c r="AJ39" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="AK39" t="s" s="2">
+      <c r="AL39" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>241</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5766,13 +5762,13 @@
         <v>50</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K40" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="L40" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5823,7 +5819,7 @@
         <v>42</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5838,18 +5834,18 @@
         <v>42</v>
       </c>
       <c r="AJ40" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>247</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5875,13 +5871,13 @@
         <v>155</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>251</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -5931,7 +5927,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5946,18 +5942,18 @@
         <v>42</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AK41" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="AK41" t="s" s="2">
+      <c r="AL41" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>254</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5980,16 +5976,16 @@
         <v>42</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6039,7 +6035,7 @@
         <v>42</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6054,22 +6050,22 @@
         <v>42</v>
       </c>
       <c r="AJ42" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL42" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6091,13 +6087,13 @@
         <v>178</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6126,11 +6122,11 @@
         <v>182</v>
       </c>
       <c r="X43" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="Y43" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="Y43" t="s" s="2">
-        <v>268</v>
-      </c>
       <c r="Z43" t="s" s="2">
         <v>42</v>
       </c>
@@ -6147,7 +6143,7 @@
         <v>42</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -6162,18 +6158,18 @@
         <v>42</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AK43" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="AK43" t="s" s="2">
+      <c r="AL43" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>271</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6199,10 +6195,10 @@
         <v>134</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6253,7 +6249,7 @@
         <v>42</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6268,7 +6264,7 @@
         <v>138</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>42</v>
@@ -6279,7 +6275,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6385,7 +6381,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6493,7 +6489,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6601,11 +6597,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6624,16 +6620,16 @@
         <v>42</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>283</v>
-      </c>
       <c r="M48" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6683,7 +6679,7 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>49</v>
@@ -6698,18 +6694,18 @@
         <v>42</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>285</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6735,10 +6731,10 @@
         <v>178</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6768,11 +6764,11 @@
         <v>182</v>
       </c>
       <c r="X49" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>42</v>
       </c>
@@ -6789,7 +6785,7 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6815,7 +6811,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6838,13 +6834,13 @@
         <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="K50" t="s" s="2">
+      <c r="L50" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6895,7 +6891,7 @@
         <v>42</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6910,7 +6906,7 @@
         <v>42</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>42</v>
@@ -6921,7 +6917,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6944,16 +6940,16 @@
         <v>42</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7003,7 +6999,7 @@
         <v>42</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7018,7 +7014,7 @@
         <v>42</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>42</v>
@@ -7029,7 +7025,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7055,13 +7051,13 @@
         <v>134</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7111,7 +7107,7 @@
         <v>42</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7126,7 +7122,7 @@
         <v>138</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>42</v>
@@ -7137,7 +7133,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7243,7 +7239,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7347,10 +7343,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="B55" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>42</v>
@@ -7372,13 +7368,13 @@
         <v>42</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7455,10 +7451,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s" s="2">
         <v>42</v>
@@ -7480,13 +7476,13 @@
         <v>42</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7563,7 +7559,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7671,7 +7667,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7697,10 +7693,10 @@
         <v>117</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7751,7 +7747,7 @@
         <v>42</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7772,12 +7768,12 @@
         <v>42</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7800,13 +7796,13 @@
         <v>42</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7857,7 +7853,7 @@
         <v>42</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7872,7 +7868,7 @@
         <v>42</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>42</v>
@@ -7883,7 +7879,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7909,10 +7905,10 @@
         <v>178</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>328</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -7942,11 +7938,11 @@
         <v>182</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>331</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>42</v>
       </c>
@@ -7963,7 +7959,7 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
@@ -7978,18 +7974,18 @@
         <v>42</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>333</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8015,10 +8011,10 @@
         <v>178</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8048,11 +8044,11 @@
         <v>189</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>42</v>
       </c>
@@ -8069,7 +8065,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8090,12 +8086,12 @@
         <v>42</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8121,16 +8117,16 @@
         <v>178</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
@@ -8158,11 +8154,11 @@
         <v>189</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>346</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>42</v>
       </c>
@@ -8179,7 +8175,7 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8194,18 +8190,18 @@
         <v>42</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>348</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8231,10 +8227,10 @@
         <v>178</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8264,11 +8260,11 @@
         <v>182</v>
       </c>
       <c r="X63" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="Y63" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="Y63" t="s" s="2">
-        <v>353</v>
-      </c>
       <c r="Z63" t="s" s="2">
         <v>42</v>
       </c>
@@ -8285,7 +8281,7 @@
         <v>42</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8300,18 +8296,18 @@
         <v>42</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL63" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>355</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8337,10 +8333,10 @@
         <v>178</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8370,11 +8366,11 @@
         <v>182</v>
       </c>
       <c r="X64" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="Y64" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="Y64" t="s" s="2">
-        <v>360</v>
-      </c>
       <c r="Z64" t="s" s="2">
         <v>42</v>
       </c>
@@ -8391,7 +8387,7 @@
         <v>42</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8406,18 +8402,18 @@
         <v>42</v>
       </c>
       <c r="AJ64" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>362</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8440,13 +8436,13 @@
         <v>42</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8497,7 +8493,7 @@
         <v>42</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8512,18 +8508,18 @@
         <v>42</v>
       </c>
       <c r="AJ65" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL65" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>367</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8549,10 +8545,10 @@
         <v>178</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8582,11 +8578,11 @@
         <v>189</v>
       </c>
       <c r="X66" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="Y66" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="Y66" t="s" s="2">
-        <v>372</v>
-      </c>
       <c r="Z66" t="s" s="2">
         <v>42</v>
       </c>
@@ -8603,7 +8599,7 @@
         <v>42</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8618,18 +8614,18 @@
         <v>42</v>
       </c>
       <c r="AJ66" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8735,7 +8731,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8808,7 +8804,7 @@
         <v>97</v>
       </c>
       <c r="AB68" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AC68" t="s" s="2">
         <v>42</v>
@@ -8843,7 +8839,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8869,16 +8865,16 @@
         <v>159</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8915,7 +8911,7 @@
         <v>42</v>
       </c>
       <c r="AA69" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AB69" s="2"/>
       <c r="AC69" t="s" s="2">
@@ -8925,7 +8921,7 @@
         <v>98</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8940,21 +8936,21 @@
         <v>42</v>
       </c>
       <c r="AJ69" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL69" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>386</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C70" t="s" s="2">
         <v>42</v>
@@ -8979,16 +8975,16 @@
         <v>159</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M70" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="N70" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9017,7 +9013,7 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>42</v>
@@ -9035,7 +9031,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9050,18 +9046,18 @@
         <v>42</v>
       </c>
       <c r="AJ70" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL70" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>386</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9087,16 +9083,16 @@
         <v>141</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9145,7 +9141,7 @@
         <v>42</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9160,18 +9156,18 @@
         <v>42</v>
       </c>
       <c r="AJ71" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>397</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9197,13 +9193,13 @@
         <v>134</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9253,7 +9249,7 @@
         <v>42</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9268,7 +9264,7 @@
         <v>138</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>42</v>
@@ -9279,7 +9275,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9385,7 +9381,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9493,7 +9489,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9601,7 +9597,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9624,13 +9620,13 @@
         <v>42</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>407</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>408</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9681,7 +9677,7 @@
         <v>42</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>49</v>
@@ -9696,18 +9692,18 @@
         <v>42</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK76" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>410</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9733,13 +9729,13 @@
         <v>68</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9768,11 +9764,11 @@
         <v>127</v>
       </c>
       <c r="X77" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="Y77" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>416</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>42</v>
       </c>
@@ -9789,7 +9785,7 @@
         <v>42</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>40</v>
@@ -9804,7 +9800,7 @@
         <v>42</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>42</v>
@@ -9815,7 +9811,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9841,10 +9837,10 @@
         <v>155</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9895,7 +9891,7 @@
         <v>42</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>40</v>
@@ -9910,7 +9906,7 @@
         <v>42</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>42</v>
@@ -9921,7 +9917,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9944,13 +9940,13 @@
         <v>42</v>
       </c>
       <c r="J79" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="K79" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="K79" t="s" s="2">
+      <c r="L79" t="s" s="2">
         <v>423</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>424</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10001,7 +9997,7 @@
         <v>42</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>40</v>
@@ -10016,18 +10012,18 @@
         <v>42</v>
       </c>
       <c r="AJ79" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AK79" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL79" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10050,16 +10046,16 @@
         <v>42</v>
       </c>
       <c r="J80" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="K80" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="K80" t="s" s="2">
+      <c r="L80" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10109,7 +10105,7 @@
         <v>42</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>40</v>
@@ -10124,7 +10120,7 @@
         <v>42</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>42</v>

</xml_diff>

<commit_message>
Build SML after updating the terminology following requirements changes in the SML FHIR IG.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/encounter-es-1.xlsx
+++ b/output/SharedMedicinesList/encounter-es-1.xlsx
@@ -595,7 +595,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/encounter-type-1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/medicines-review-type-2</t>
   </si>
   <si>
     <t>.code</t>
@@ -1470,7 +1470,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="72.9921875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="63.2421875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="68.2734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>

</xml_diff>